<commit_message>
chore: update main pages
</commit_message>
<xml_diff>
--- a/main/kdl-ihe-classcode.xlsx
+++ b/main/kdl-ihe-classcode.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="1030">
   <si>
     <t>Property</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2025.0.1</t>
+    <t>2026.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-01</t>
+    <t>2026-01-01</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -94,7 +94,7 @@
     <t>Copyright</t>
   </si>
   <si>
-    <t>2025 DVMD e.V.</t>
+    <t>2026 DVMD e.V.</t>
   </si>
   <si>
     <t>Source</t>
@@ -811,6 +811,12 @@
     <t>Patientenbild</t>
   </si>
   <si>
+    <t>AM160114</t>
+  </si>
+  <si>
+    <t>Anästhesieausweis</t>
+  </si>
+  <si>
     <t>AM160199</t>
   </si>
   <si>
@@ -1249,6 +1255,12 @@
     <t>Checkliste bildgebende Diagnostik</t>
   </si>
   <si>
+    <t>DG020116</t>
+  </si>
+  <si>
+    <t>Zugangscode Bildportal</t>
+  </si>
+  <si>
     <t>DG020199</t>
   </si>
   <si>
@@ -2549,6 +2561,12 @@
   </si>
   <si>
     <t>IPSS (Internationaler Prostata Symptom Score)</t>
+  </si>
+  <si>
+    <t>VL010109</t>
+  </si>
+  <si>
+    <t>Sepsisdokumentation</t>
   </si>
   <si>
     <t>VL010199</t>
@@ -3362,7 +3380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E450"/>
+  <dimension ref="A1:E453"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5198,10 +5216,10 @@
         <v>37</v>
       </c>
       <c r="D108" t="s" s="2">
-        <v>80</v>
+        <v>239</v>
       </c>
       <c r="E108" t="s" s="2">
-        <v>81</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109">
@@ -5283,10 +5301,10 @@
         <v>37</v>
       </c>
       <c r="D113" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E113" t="s" s="2">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114">
@@ -5351,10 +5369,10 @@
         <v>37</v>
       </c>
       <c r="D117" t="s" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E117" t="s" s="2">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="118">
@@ -5368,27 +5386,27 @@
         <v>37</v>
       </c>
       <c r="D118" t="s" s="2">
-        <v>287</v>
+        <v>80</v>
       </c>
       <c r="E118" t="s" s="2">
-        <v>288</v>
+        <v>81</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="B119" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="C119" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D119" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="B119" t="s" s="2">
+      <c r="E119" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="C119" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D119" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="E119" t="s" s="2">
-        <v>288</v>
       </c>
     </row>
     <row r="120">
@@ -5402,10 +5420,10 @@
         <v>37</v>
       </c>
       <c r="D120" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E120" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="121">
@@ -5419,10 +5437,10 @@
         <v>37</v>
       </c>
       <c r="D121" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E121" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="122">
@@ -5436,10 +5454,10 @@
         <v>37</v>
       </c>
       <c r="D122" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E122" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123">
@@ -5453,10 +5471,10 @@
         <v>37</v>
       </c>
       <c r="D123" t="s" s="2">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="E123" t="s" s="2">
-        <v>81</v>
+        <v>290</v>
       </c>
     </row>
     <row r="124">
@@ -5572,10 +5590,10 @@
         <v>37</v>
       </c>
       <c r="D130" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E130" t="s" s="2">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="131">
@@ -5589,10 +5607,10 @@
         <v>37</v>
       </c>
       <c r="D131" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E131" t="s" s="2">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="132">
@@ -5878,10 +5896,10 @@
         <v>37</v>
       </c>
       <c r="D148" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E148" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="149">
@@ -5895,10 +5913,10 @@
         <v>37</v>
       </c>
       <c r="D149" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E149" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="150">
@@ -5929,10 +5947,10 @@
         <v>37</v>
       </c>
       <c r="D151" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E151" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="152">
@@ -5946,10 +5964,10 @@
         <v>37</v>
       </c>
       <c r="D152" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E152" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="153">
@@ -5963,10 +5981,10 @@
         <v>37</v>
       </c>
       <c r="D153" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E153" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="154">
@@ -5980,10 +5998,10 @@
         <v>37</v>
       </c>
       <c r="D154" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E154" t="s" s="2">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="155">
@@ -6048,10 +6066,10 @@
         <v>37</v>
       </c>
       <c r="D158" t="s" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E158" t="s" s="2">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="159">
@@ -6065,10 +6083,10 @@
         <v>37</v>
       </c>
       <c r="D159" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E159" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="160">
@@ -6116,10 +6134,10 @@
         <v>37</v>
       </c>
       <c r="D162" t="s" s="2">
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="E162" t="s" s="2">
-        <v>240</v>
+        <v>89</v>
       </c>
     </row>
     <row r="163">
@@ -6133,10 +6151,10 @@
         <v>37</v>
       </c>
       <c r="D163" t="s" s="2">
-        <v>147</v>
+        <v>239</v>
       </c>
       <c r="E163" t="s" s="2">
-        <v>148</v>
+        <v>240</v>
       </c>
     </row>
     <row r="164">
@@ -6150,10 +6168,10 @@
         <v>37</v>
       </c>
       <c r="D164" t="s" s="2">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E164" t="s" s="2">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="165">
@@ -6167,10 +6185,10 @@
         <v>37</v>
       </c>
       <c r="D165" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E165" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="166">
@@ -6184,10 +6202,10 @@
         <v>37</v>
       </c>
       <c r="D166" t="s" s="2">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="E166" t="s" s="2">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="167">
@@ -6252,10 +6270,10 @@
         <v>37</v>
       </c>
       <c r="D170" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E170" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="171">
@@ -6269,10 +6287,10 @@
         <v>37</v>
       </c>
       <c r="D171" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E171" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="172">
@@ -6405,10 +6423,10 @@
         <v>37</v>
       </c>
       <c r="D179" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E179" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="180">
@@ -6422,10 +6440,10 @@
         <v>37</v>
       </c>
       <c r="D180" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E180" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="181">
@@ -6439,10 +6457,10 @@
         <v>37</v>
       </c>
       <c r="D181" t="s" s="2">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="E181" t="s" s="2">
-        <v>123</v>
+        <v>81</v>
       </c>
     </row>
     <row r="182">
@@ -6473,10 +6491,10 @@
         <v>37</v>
       </c>
       <c r="D183" t="s" s="2">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="E183" t="s" s="2">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="184">
@@ -6490,10 +6508,10 @@
         <v>37</v>
       </c>
       <c r="D184" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E184" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="185">
@@ -6507,10 +6525,10 @@
         <v>37</v>
       </c>
       <c r="D185" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E185" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="186">
@@ -6524,10 +6542,10 @@
         <v>37</v>
       </c>
       <c r="D186" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E186" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="187">
@@ -6575,10 +6593,10 @@
         <v>37</v>
       </c>
       <c r="D189" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E189" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="190">
@@ -6728,10 +6746,10 @@
         <v>37</v>
       </c>
       <c r="D198" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E198" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="199">
@@ -6762,10 +6780,10 @@
         <v>37</v>
       </c>
       <c r="D200" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E200" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="201">
@@ -6796,10 +6814,10 @@
         <v>37</v>
       </c>
       <c r="D202" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E202" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="203">
@@ -6830,10 +6848,10 @@
         <v>37</v>
       </c>
       <c r="D204" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E204" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="205">
@@ -6898,10 +6916,10 @@
         <v>37</v>
       </c>
       <c r="D208" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E208" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="209">
@@ -6932,10 +6950,10 @@
         <v>37</v>
       </c>
       <c r="D210" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E210" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="211">
@@ -6983,10 +7001,10 @@
         <v>37</v>
       </c>
       <c r="D213" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E213" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="214">
@@ -7000,44 +7018,44 @@
         <v>37</v>
       </c>
       <c r="D214" t="s" s="2">
-        <v>481</v>
+        <v>56</v>
       </c>
       <c r="E214" t="s" s="2">
-        <v>482</v>
+        <v>57</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s" s="2">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B215" t="s" s="2">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C215" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D215" t="s" s="2">
-        <v>481</v>
+        <v>88</v>
       </c>
       <c r="E215" t="s" s="2">
-        <v>482</v>
+        <v>89</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="B216" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="C216" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D216" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="B216" t="s" s="2">
+      <c r="E216" t="s" s="2">
         <v>486</v>
-      </c>
-      <c r="C216" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D216" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="E216" t="s" s="2">
-        <v>482</v>
       </c>
     </row>
     <row r="217">
@@ -7051,44 +7069,44 @@
         <v>37</v>
       </c>
       <c r="D217" t="s" s="2">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E217" t="s" s="2">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s" s="2">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B218" t="s" s="2">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C218" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D218" t="s" s="2">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="E218" t="s" s="2">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="B219" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="C219" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D219" t="s" s="2">
         <v>493</v>
       </c>
-      <c r="B219" t="s" s="2">
+      <c r="E219" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="C219" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D219" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="E219" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="220">
@@ -7102,10 +7120,10 @@
         <v>37</v>
       </c>
       <c r="D220" t="s" s="2">
-        <v>239</v>
+        <v>485</v>
       </c>
       <c r="E220" t="s" s="2">
-        <v>240</v>
+        <v>486</v>
       </c>
     </row>
     <row r="221">
@@ -7136,10 +7154,10 @@
         <v>37</v>
       </c>
       <c r="D222" t="s" s="2">
-        <v>38</v>
+        <v>239</v>
       </c>
       <c r="E222" t="s" s="2">
-        <v>39</v>
+        <v>240</v>
       </c>
     </row>
     <row r="223">
@@ -7153,10 +7171,10 @@
         <v>37</v>
       </c>
       <c r="D223" t="s" s="2">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="E223" t="s" s="2">
-        <v>240</v>
+        <v>93</v>
       </c>
     </row>
     <row r="224">
@@ -7170,10 +7188,10 @@
         <v>37</v>
       </c>
       <c r="D224" t="s" s="2">
-        <v>239</v>
+        <v>38</v>
       </c>
       <c r="E224" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225">
@@ -7187,10 +7205,10 @@
         <v>37</v>
       </c>
       <c r="D225" t="s" s="2">
-        <v>80</v>
+        <v>239</v>
       </c>
       <c r="E225" t="s" s="2">
-        <v>81</v>
+        <v>240</v>
       </c>
     </row>
     <row r="226">
@@ -7204,10 +7222,10 @@
         <v>37</v>
       </c>
       <c r="D226" t="s" s="2">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="E226" t="s" s="2">
-        <v>77</v>
+        <v>240</v>
       </c>
     </row>
     <row r="227">
@@ -7221,10 +7239,10 @@
         <v>37</v>
       </c>
       <c r="D227" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E227" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="228">
@@ -7238,10 +7256,10 @@
         <v>37</v>
       </c>
       <c r="D228" t="s" s="2">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="E228" t="s" s="2">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="229">
@@ -7255,10 +7273,10 @@
         <v>37</v>
       </c>
       <c r="D229" t="s" s="2">
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="E229" t="s" s="2">
-        <v>240</v>
+        <v>89</v>
       </c>
     </row>
     <row r="230">
@@ -7306,10 +7324,10 @@
         <v>37</v>
       </c>
       <c r="D232" t="s" s="2">
-        <v>239</v>
+        <v>38</v>
       </c>
       <c r="E232" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
     </row>
     <row r="233">
@@ -7340,10 +7358,10 @@
         <v>37</v>
       </c>
       <c r="D234" t="s" s="2">
-        <v>38</v>
+        <v>239</v>
       </c>
       <c r="E234" t="s" s="2">
-        <v>39</v>
+        <v>240</v>
       </c>
     </row>
     <row r="235">
@@ -7357,10 +7375,10 @@
         <v>37</v>
       </c>
       <c r="D235" t="s" s="2">
-        <v>102</v>
+        <v>239</v>
       </c>
       <c r="E235" t="s" s="2">
-        <v>103</v>
+        <v>240</v>
       </c>
     </row>
     <row r="236">
@@ -7374,10 +7392,10 @@
         <v>37</v>
       </c>
       <c r="D236" t="s" s="2">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E236" t="s" s="2">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="237">
@@ -7408,10 +7426,10 @@
         <v>37</v>
       </c>
       <c r="D238" t="s" s="2">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="E238" t="s" s="2">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="239">
@@ -7442,10 +7460,10 @@
         <v>37</v>
       </c>
       <c r="D240" t="s" s="2">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E240" t="s" s="2">
-        <v>57</v>
+        <v>103</v>
       </c>
     </row>
     <row r="241">
@@ -7476,10 +7494,10 @@
         <v>37</v>
       </c>
       <c r="D242" t="s" s="2">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="E242" t="s" s="2">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="243">
@@ -7527,44 +7545,44 @@
         <v>37</v>
       </c>
       <c r="D245" t="s" s="2">
-        <v>547</v>
+        <v>102</v>
       </c>
       <c r="E245" t="s" s="2">
-        <v>548</v>
+        <v>103</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s" s="2">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B246" t="s" s="2">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C246" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D246" t="s" s="2">
-        <v>547</v>
+        <v>102</v>
       </c>
       <c r="E246" t="s" s="2">
-        <v>548</v>
+        <v>103</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="B247" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="C247" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D247" t="s" s="2">
         <v>551</v>
       </c>
-      <c r="B247" t="s" s="2">
+      <c r="E247" t="s" s="2">
         <v>552</v>
-      </c>
-      <c r="C247" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D247" t="s" s="2">
-        <v>547</v>
-      </c>
-      <c r="E247" t="s" s="2">
-        <v>548</v>
       </c>
     </row>
     <row r="248">
@@ -7578,10 +7596,10 @@
         <v>37</v>
       </c>
       <c r="D248" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E248" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="249">
@@ -7595,10 +7613,10 @@
         <v>37</v>
       </c>
       <c r="D249" t="s" s="2">
-        <v>102</v>
+        <v>551</v>
       </c>
       <c r="E249" t="s" s="2">
-        <v>103</v>
+        <v>552</v>
       </c>
     </row>
     <row r="250">
@@ -7612,10 +7630,10 @@
         <v>37</v>
       </c>
       <c r="D250" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E250" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="251">
@@ -7629,10 +7647,10 @@
         <v>37</v>
       </c>
       <c r="D251" t="s" s="2">
-        <v>547</v>
+        <v>102</v>
       </c>
       <c r="E251" t="s" s="2">
-        <v>548</v>
+        <v>103</v>
       </c>
     </row>
     <row r="252">
@@ -7646,10 +7664,10 @@
         <v>37</v>
       </c>
       <c r="D252" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E252" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="253">
@@ -7663,10 +7681,10 @@
         <v>37</v>
       </c>
       <c r="D253" t="s" s="2">
-        <v>122</v>
+        <v>551</v>
       </c>
       <c r="E253" t="s" s="2">
-        <v>123</v>
+        <v>552</v>
       </c>
     </row>
     <row r="254">
@@ -7680,10 +7698,10 @@
         <v>37</v>
       </c>
       <c r="D254" t="s" s="2">
-        <v>76</v>
+        <v>551</v>
       </c>
       <c r="E254" t="s" s="2">
-        <v>77</v>
+        <v>552</v>
       </c>
     </row>
     <row r="255">
@@ -7697,10 +7715,10 @@
         <v>37</v>
       </c>
       <c r="D255" t="s" s="2">
-        <v>547</v>
+        <v>122</v>
       </c>
       <c r="E255" t="s" s="2">
-        <v>548</v>
+        <v>123</v>
       </c>
     </row>
     <row r="256">
@@ -7714,10 +7732,10 @@
         <v>37</v>
       </c>
       <c r="D256" t="s" s="2">
-        <v>547</v>
+        <v>76</v>
       </c>
       <c r="E256" t="s" s="2">
-        <v>548</v>
+        <v>77</v>
       </c>
     </row>
     <row r="257">
@@ -7731,10 +7749,10 @@
         <v>37</v>
       </c>
       <c r="D257" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E257" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="258">
@@ -7748,10 +7766,10 @@
         <v>37</v>
       </c>
       <c r="D258" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E258" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="259">
@@ -7765,10 +7783,10 @@
         <v>37</v>
       </c>
       <c r="D259" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E259" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="260">
@@ -7782,10 +7800,10 @@
         <v>37</v>
       </c>
       <c r="D260" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E260" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="261">
@@ -7799,10 +7817,10 @@
         <v>37</v>
       </c>
       <c r="D261" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="E261" t="s" s="2">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="262">
@@ -7816,10 +7834,10 @@
         <v>37</v>
       </c>
       <c r="D262" t="s" s="2">
-        <v>88</v>
+        <v>551</v>
       </c>
       <c r="E262" t="s" s="2">
-        <v>89</v>
+        <v>552</v>
       </c>
     </row>
     <row r="263">
@@ -7833,10 +7851,10 @@
         <v>37</v>
       </c>
       <c r="D263" t="s" s="2">
-        <v>88</v>
+        <v>551</v>
       </c>
       <c r="E263" t="s" s="2">
-        <v>89</v>
+        <v>552</v>
       </c>
     </row>
     <row r="264">
@@ -7901,10 +7919,10 @@
         <v>37</v>
       </c>
       <c r="D267" t="s" s="2">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E267" t="s" s="2">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="268">
@@ -7935,10 +7953,10 @@
         <v>37</v>
       </c>
       <c r="D269" t="s" s="2">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="E269" t="s" s="2">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="270">
@@ -7969,10 +7987,10 @@
         <v>37</v>
       </c>
       <c r="D271" t="s" s="2">
-        <v>481</v>
+        <v>122</v>
       </c>
       <c r="E271" t="s" s="2">
-        <v>482</v>
+        <v>123</v>
       </c>
     </row>
     <row r="272">
@@ -8003,10 +8021,10 @@
         <v>37</v>
       </c>
       <c r="D273" t="s" s="2">
-        <v>88</v>
+        <v>485</v>
       </c>
       <c r="E273" t="s" s="2">
-        <v>89</v>
+        <v>486</v>
       </c>
     </row>
     <row r="274">
@@ -8020,10 +8038,10 @@
         <v>37</v>
       </c>
       <c r="D274" t="s" s="2">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E274" t="s" s="2">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="275">
@@ -8054,10 +8072,10 @@
         <v>37</v>
       </c>
       <c r="D276" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E276" t="s" s="2">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="277">
@@ -8122,10 +8140,10 @@
         <v>37</v>
       </c>
       <c r="D280" t="s" s="2">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E280" t="s" s="2">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="281">
@@ -8139,10 +8157,10 @@
         <v>37</v>
       </c>
       <c r="D281" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E281" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="282">
@@ -8156,10 +8174,10 @@
         <v>37</v>
       </c>
       <c r="D282" t="s" s="2">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E282" t="s" s="2">
-        <v>57</v>
+        <v>103</v>
       </c>
     </row>
     <row r="283">
@@ -8207,10 +8225,10 @@
         <v>37</v>
       </c>
       <c r="D285" t="s" s="2">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="E285" t="s" s="2">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="286">
@@ -8224,10 +8242,10 @@
         <v>37</v>
       </c>
       <c r="D286" t="s" s="2">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="E286" t="s" s="2">
-        <v>123</v>
+        <v>57</v>
       </c>
     </row>
     <row r="287">
@@ -8258,10 +8276,10 @@
         <v>37</v>
       </c>
       <c r="D288" t="s" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E288" t="s" s="2">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="289">
@@ -8275,10 +8293,10 @@
         <v>37</v>
       </c>
       <c r="D289" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E289" t="s" s="2">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="290">
@@ -8445,10 +8463,10 @@
         <v>37</v>
       </c>
       <c r="D299" t="s" s="2">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="E299" t="s" s="2">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="300">
@@ -8479,10 +8497,10 @@
         <v>37</v>
       </c>
       <c r="D301" t="s" s="2">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="E301" t="s" s="2">
-        <v>148</v>
+        <v>39</v>
       </c>
     </row>
     <row r="302">
@@ -8496,10 +8514,10 @@
         <v>37</v>
       </c>
       <c r="D302" t="s" s="2">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="E302" t="s" s="2">
-        <v>148</v>
+        <v>89</v>
       </c>
     </row>
     <row r="303">
@@ -8507,7 +8525,7 @@
         <v>663</v>
       </c>
       <c r="B303" t="s" s="2">
-        <v>378</v>
+        <v>664</v>
       </c>
       <c r="C303" t="s" s="2">
         <v>37</v>
@@ -8521,10 +8539,10 @@
     </row>
     <row r="304">
       <c r="A304" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B304" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C304" t="s" s="2">
         <v>37</v>
@@ -8538,10 +8556,10 @@
     </row>
     <row r="305">
       <c r="A305" t="s" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B305" t="s" s="2">
-        <v>667</v>
+        <v>380</v>
       </c>
       <c r="C305" t="s" s="2">
         <v>37</v>
@@ -8615,10 +8633,10 @@
         <v>37</v>
       </c>
       <c r="D309" t="s" s="2">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="E309" t="s" s="2">
-        <v>103</v>
+        <v>148</v>
       </c>
     </row>
     <row r="310">
@@ -8632,10 +8650,10 @@
         <v>37</v>
       </c>
       <c r="D310" t="s" s="2">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E310" t="s" s="2">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="311">
@@ -8649,10 +8667,10 @@
         <v>37</v>
       </c>
       <c r="D311" t="s" s="2">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E311" t="s" s="2">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="312">
@@ -8768,10 +8786,10 @@
         <v>37</v>
       </c>
       <c r="D318" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E318" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="319">
@@ -8785,10 +8803,10 @@
         <v>37</v>
       </c>
       <c r="D319" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E319" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="320">
@@ -8853,10 +8871,10 @@
         <v>37</v>
       </c>
       <c r="D323" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E323" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="324">
@@ -8881,7 +8899,7 @@
         <v>706</v>
       </c>
       <c r="B325" t="s" s="2">
-        <v>133</v>
+        <v>707</v>
       </c>
       <c r="C325" t="s" s="2">
         <v>37</v>
@@ -8895,27 +8913,27 @@
     </row>
     <row r="326">
       <c r="A326" t="s" s="2">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B326" t="s" s="2">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C326" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D326" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E326" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="s" s="2">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B327" t="s" s="2">
-        <v>710</v>
+        <v>133</v>
       </c>
       <c r="C327" t="s" s="2">
         <v>37</v>
@@ -8938,10 +8956,10 @@
         <v>37</v>
       </c>
       <c r="D328" t="s" s="2">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E328" t="s" s="2">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="329">
@@ -8972,10 +8990,10 @@
         <v>37</v>
       </c>
       <c r="D330" t="s" s="2">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E330" t="s" s="2">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="331">
@@ -9006,10 +9024,10 @@
         <v>37</v>
       </c>
       <c r="D332" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E332" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="333">
@@ -9074,10 +9092,10 @@
         <v>37</v>
       </c>
       <c r="D336" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E336" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="337">
@@ -9108,10 +9126,10 @@
         <v>37</v>
       </c>
       <c r="D338" t="s" s="2">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="E338" t="s" s="2">
-        <v>148</v>
+        <v>81</v>
       </c>
     </row>
     <row r="339">
@@ -9125,10 +9143,10 @@
         <v>37</v>
       </c>
       <c r="D339" t="s" s="2">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="E339" t="s" s="2">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="340">
@@ -9142,10 +9160,10 @@
         <v>37</v>
       </c>
       <c r="D340" t="s" s="2">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E340" t="s" s="2">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="341">
@@ -9159,44 +9177,44 @@
         <v>37</v>
       </c>
       <c r="D341" t="s" s="2">
-        <v>739</v>
+        <v>38</v>
       </c>
       <c r="E341" t="s" s="2">
-        <v>740</v>
+        <v>39</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="s" s="2">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B342" t="s" s="2">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C342" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D342" t="s" s="2">
-        <v>739</v>
+        <v>88</v>
       </c>
       <c r="E342" t="s" s="2">
-        <v>740</v>
+        <v>89</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="s" s="2">
+        <v>741</v>
+      </c>
+      <c r="B343" t="s" s="2">
+        <v>742</v>
+      </c>
+      <c r="C343" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D343" t="s" s="2">
         <v>743</v>
       </c>
-      <c r="B343" t="s" s="2">
+      <c r="E343" t="s" s="2">
         <v>744</v>
-      </c>
-      <c r="C343" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D343" t="s" s="2">
-        <v>739</v>
-      </c>
-      <c r="E343" t="s" s="2">
-        <v>740</v>
       </c>
     </row>
     <row r="344">
@@ -9210,10 +9228,10 @@
         <v>37</v>
       </c>
       <c r="D344" t="s" s="2">
-        <v>80</v>
+        <v>743</v>
       </c>
       <c r="E344" t="s" s="2">
-        <v>81</v>
+        <v>744</v>
       </c>
     </row>
     <row r="345">
@@ -9227,10 +9245,10 @@
         <v>37</v>
       </c>
       <c r="D345" t="s" s="2">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="E345" t="s" s="2">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="346">
@@ -9244,10 +9262,10 @@
         <v>37</v>
       </c>
       <c r="D346" t="s" s="2">
-        <v>739</v>
+        <v>80</v>
       </c>
       <c r="E346" t="s" s="2">
-        <v>740</v>
+        <v>81</v>
       </c>
     </row>
     <row r="347">
@@ -9261,10 +9279,10 @@
         <v>37</v>
       </c>
       <c r="D347" t="s" s="2">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="E347" t="s" s="2">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="348">
@@ -9278,10 +9296,10 @@
         <v>37</v>
       </c>
       <c r="D348" t="s" s="2">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="E348" t="s" s="2">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="349">
@@ -9295,10 +9313,10 @@
         <v>37</v>
       </c>
       <c r="D349" t="s" s="2">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="E349" t="s" s="2">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="350">
@@ -9312,10 +9330,10 @@
         <v>37</v>
       </c>
       <c r="D350" t="s" s="2">
-        <v>92</v>
+        <v>743</v>
       </c>
       <c r="E350" t="s" s="2">
-        <v>93</v>
+        <v>744</v>
       </c>
     </row>
     <row r="351">
@@ -9329,10 +9347,10 @@
         <v>37</v>
       </c>
       <c r="D351" t="s" s="2">
-        <v>88</v>
+        <v>743</v>
       </c>
       <c r="E351" t="s" s="2">
-        <v>89</v>
+        <v>744</v>
       </c>
     </row>
     <row r="352">
@@ -9346,10 +9364,10 @@
         <v>37</v>
       </c>
       <c r="D352" t="s" s="2">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="E352" t="s" s="2">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
     <row r="353">
@@ -9380,10 +9398,10 @@
         <v>37</v>
       </c>
       <c r="D354" t="s" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E354" t="s" s="2">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="355">
@@ -9465,10 +9483,10 @@
         <v>37</v>
       </c>
       <c r="D359" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E359" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="360">
@@ -9499,10 +9517,10 @@
         <v>37</v>
       </c>
       <c r="D361" t="s" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E361" t="s" s="2">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="362">
@@ -9533,10 +9551,10 @@
         <v>37</v>
       </c>
       <c r="D363" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E363" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="364">
@@ -9550,10 +9568,10 @@
         <v>37</v>
       </c>
       <c r="D364" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E364" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="365">
@@ -9567,10 +9585,10 @@
         <v>37</v>
       </c>
       <c r="D365" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E365" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="366">
@@ -9584,10 +9602,10 @@
         <v>37</v>
       </c>
       <c r="D366" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E366" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="367">
@@ -9601,10 +9619,10 @@
         <v>37</v>
       </c>
       <c r="D367" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E367" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="368">
@@ -9618,10 +9636,10 @@
         <v>37</v>
       </c>
       <c r="D368" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E368" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="369">
@@ -9652,10 +9670,10 @@
         <v>37</v>
       </c>
       <c r="D370" t="s" s="2">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E370" t="s" s="2">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="371">
@@ -9669,10 +9687,10 @@
         <v>37</v>
       </c>
       <c r="D371" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E371" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="372">
@@ -9686,10 +9704,10 @@
         <v>37</v>
       </c>
       <c r="D372" t="s" s="2">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E372" t="s" s="2">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="373">
@@ -9788,10 +9806,10 @@
         <v>37</v>
       </c>
       <c r="D378" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E378" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="379">
@@ -9822,10 +9840,10 @@
         <v>37</v>
       </c>
       <c r="D380" t="s" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E380" t="s" s="2">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="381">
@@ -9839,10 +9857,10 @@
         <v>37</v>
       </c>
       <c r="D381" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E381" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="382">
@@ -9873,10 +9891,10 @@
         <v>37</v>
       </c>
       <c r="D383" t="s" s="2">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="E383" t="s" s="2">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="384">
@@ -9907,10 +9925,10 @@
         <v>37</v>
       </c>
       <c r="D385" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E385" t="s" s="2">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="386">
@@ -9924,10 +9942,10 @@
         <v>37</v>
       </c>
       <c r="D386" t="s" s="2">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="E386" t="s" s="2">
-        <v>148</v>
+        <v>89</v>
       </c>
     </row>
     <row r="387">
@@ -9941,10 +9959,10 @@
         <v>37</v>
       </c>
       <c r="D387" t="s" s="2">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="E387" t="s" s="2">
-        <v>148</v>
+        <v>81</v>
       </c>
     </row>
     <row r="388">
@@ -10077,10 +10095,10 @@
         <v>37</v>
       </c>
       <c r="D395" t="s" s="2">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="E395" t="s" s="2">
-        <v>39</v>
+        <v>148</v>
       </c>
     </row>
     <row r="396">
@@ -10094,10 +10112,10 @@
         <v>37</v>
       </c>
       <c r="D396" t="s" s="2">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="E396" t="s" s="2">
-        <v>93</v>
+        <v>148</v>
       </c>
     </row>
     <row r="397">
@@ -10111,10 +10129,10 @@
         <v>37</v>
       </c>
       <c r="D397" t="s" s="2">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="E397" t="s" s="2">
-        <v>81</v>
+        <v>148</v>
       </c>
     </row>
     <row r="398">
@@ -10128,10 +10146,10 @@
         <v>37</v>
       </c>
       <c r="D398" t="s" s="2">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="E398" t="s" s="2">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="399">
@@ -10145,10 +10163,10 @@
         <v>37</v>
       </c>
       <c r="D399" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E399" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="400">
@@ -10179,10 +10197,10 @@
         <v>37</v>
       </c>
       <c r="D401" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E401" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="402">
@@ -10196,10 +10214,10 @@
         <v>37</v>
       </c>
       <c r="D402" t="s" s="2">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E402" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="403">
@@ -10247,10 +10265,10 @@
         <v>37</v>
       </c>
       <c r="D405" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E405" t="s" s="2">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="406">
@@ -10264,10 +10282,10 @@
         <v>37</v>
       </c>
       <c r="D406" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E406" t="s" s="2">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="407">
@@ -10281,10 +10299,10 @@
         <v>37</v>
       </c>
       <c r="D407" t="s" s="2">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E407" t="s" s="2">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="408">
@@ -10298,10 +10316,10 @@
         <v>37</v>
       </c>
       <c r="D408" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E408" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="409">
@@ -10332,10 +10350,10 @@
         <v>37</v>
       </c>
       <c r="D410" t="s" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E410" t="s" s="2">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="411">
@@ -10468,10 +10486,10 @@
         <v>37</v>
       </c>
       <c r="D418" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E418" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="419">
@@ -10519,10 +10537,10 @@
         <v>37</v>
       </c>
       <c r="D421" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E421" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="422">
@@ -10689,10 +10707,10 @@
         <v>37</v>
       </c>
       <c r="D431" t="s" s="2">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E431" t="s" s="2">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="432">
@@ -10706,10 +10724,10 @@
         <v>37</v>
       </c>
       <c r="D432" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E432" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="433">
@@ -10717,101 +10735,101 @@
         <v>923</v>
       </c>
       <c r="B433" t="s" s="2">
-        <v>705</v>
+        <v>924</v>
       </c>
       <c r="C433" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D433" t="s" s="2">
-        <v>287</v>
+        <v>88</v>
       </c>
       <c r="E433" t="s" s="2">
-        <v>288</v>
+        <v>89</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s" s="2">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B434" t="s" s="2">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C434" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D434" t="s" s="2">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E434" t="s" s="2">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s" s="2">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B435" t="s" s="2">
-        <v>510</v>
+        <v>928</v>
       </c>
       <c r="C435" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D435" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E435" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s" s="2">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="B436" t="s" s="2">
-        <v>928</v>
+        <v>709</v>
       </c>
       <c r="C436" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D436" t="s" s="2">
-        <v>88</v>
+        <v>289</v>
       </c>
       <c r="E436" t="s" s="2">
-        <v>89</v>
+        <v>290</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B437" t="s" s="2">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C437" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D437" t="s" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E437" t="s" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s" s="2">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B438" t="s" s="2">
-        <v>932</v>
+        <v>514</v>
       </c>
       <c r="C438" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D438" t="s" s="2">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="E438" t="s" s="2">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="439">
@@ -10842,10 +10860,10 @@
         <v>37</v>
       </c>
       <c r="D440" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E440" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="441">
@@ -10859,10 +10877,10 @@
         <v>37</v>
       </c>
       <c r="D441" t="s" s="2">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="E441" t="s" s="2">
-        <v>89</v>
+        <v>39</v>
       </c>
     </row>
     <row r="442">
@@ -10927,10 +10945,10 @@
         <v>37</v>
       </c>
       <c r="D445" t="s" s="2">
-        <v>481</v>
+        <v>88</v>
       </c>
       <c r="E445" t="s" s="2">
-        <v>482</v>
+        <v>89</v>
       </c>
     </row>
     <row r="446">
@@ -10961,10 +10979,10 @@
         <v>37</v>
       </c>
       <c r="D447" t="s" s="2">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E447" t="s" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="448">
@@ -10978,10 +10996,10 @@
         <v>37</v>
       </c>
       <c r="D448" t="s" s="2">
-        <v>92</v>
+        <v>485</v>
       </c>
       <c r="E448" t="s" s="2">
-        <v>93</v>
+        <v>486</v>
       </c>
     </row>
     <row r="449">
@@ -10995,10 +11013,10 @@
         <v>37</v>
       </c>
       <c r="D449" t="s" s="2">
-        <v>481</v>
+        <v>88</v>
       </c>
       <c r="E449" t="s" s="2">
-        <v>482</v>
+        <v>89</v>
       </c>
     </row>
     <row r="450">
@@ -11012,9 +11030,60 @@
         <v>37</v>
       </c>
       <c r="D450" t="s" s="2">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E450" t="s" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="s" s="2">
+        <v>957</v>
+      </c>
+      <c r="B451" t="s" s="2">
+        <v>958</v>
+      </c>
+      <c r="C451" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D451" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="E451" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="s" s="2">
+        <v>959</v>
+      </c>
+      <c r="B452" t="s" s="2">
+        <v>960</v>
+      </c>
+      <c r="C452" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D452" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="E452" t="s" s="2">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="s" s="2">
+        <v>961</v>
+      </c>
+      <c r="B453" t="s" s="2">
+        <v>962</v>
+      </c>
+      <c r="C453" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D453" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="E453" t="s" s="2">
         <v>89</v>
       </c>
     </row>
@@ -11059,7 +11128,7 @@
         <v>21</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>957</v>
+        <v>963</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>21</v>
@@ -11067,546 +11136,546 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>958</v>
+        <v>964</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>959</v>
+        <v>965</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>962</v>
+        <v>968</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>963</v>
+        <v>969</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>965</v>
+        <v>971</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>972</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>973</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s" s="2">
         <v>966</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="E6" t="s" s="2">
         <v>967</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>960</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>961</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>968</v>
+        <v>974</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>969</v>
+        <v>975</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>970</v>
+        <v>976</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>971</v>
+        <v>977</v>
       </c>
       <c r="C8" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>973</v>
+        <v>979</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>974</v>
+        <v>980</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>975</v>
+        <v>981</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>976</v>
+        <v>982</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>977</v>
+        <v>983</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>978</v>
+        <v>984</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>979</v>
+        <v>985</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>980</v>
+        <v>986</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>982</v>
+        <v>988</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>985</v>
+        <v>991</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>987</v>
+        <v>993</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>991</v>
+        <v>997</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>992</v>
+        <v>998</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>993</v>
+        <v>999</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>994</v>
+        <v>1000</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>995</v>
+        <v>1001</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>996</v>
+        <v>1002</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>997</v>
+        <v>1003</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>999</v>
+        <v>1005</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>1003</v>
+        <v>1009</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>1005</v>
+        <v>1011</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>1006</v>
+        <v>1012</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>1007</v>
+        <v>1013</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>1008</v>
+        <v>1014</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>1012</v>
+        <v>1018</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="C29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>1022</v>
+        <v>1028</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>1023</v>
+        <v>1029</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>961</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>